<commit_message>
[cvz] fixing things with mask on input
</commit_message>
<xml_diff>
--- a/main/app/cvzDoubleTouch/conf/output_port_masks/forearm_mask_generator.xlsx
+++ b/main/app/cvzDoubleTouch/conf/output_port_masks/forearm_mask_generator.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>taxel line</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>max bounds</t>
+  </si>
+  <si>
+    <t>max bounds binary</t>
   </si>
   <si>
     <t>mask</t>
@@ -124,14 +127,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:NU4"/>
+  <dimension ref="A1:NU5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="NI1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="NW4" activeCellId="0" pane="topLeft" sqref="NW4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="NG1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="NG4" activeCellId="0" pane="topLeft" sqref="NG4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -3609,1156 +3613,2313 @@
       <c r="A4" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="W4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="X4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BF4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BG4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BH4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BJ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BK4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BN4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BQ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BR4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BS4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BT4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BV4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BW4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BX4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BY4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BZ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CB4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="CC4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CD4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CE4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CF4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="CG4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CH4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CI4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CJ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CK4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CL4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CM4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CN4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CP4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CQ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CR4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="CS4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CT4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CU4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CV4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CW4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CX4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CY4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="CZ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="DA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DB4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DC4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DD4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="DE4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DF4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DG4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DH4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DI4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DJ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DK4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DL4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="DM4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DN4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DO4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DP4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="DQ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DR4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DS4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DT4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DU4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DV4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DW4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DX4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="DY4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="DZ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EB4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="EC4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="ED4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EE4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EF4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EG4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EH4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EI4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EJ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="EK4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EL4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EM4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EN4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="EO4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EP4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EQ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="ER4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="ES4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="ET4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EU4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EV4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="EW4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EX4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EY4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="EZ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="FA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FB4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FC4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FD4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FE4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FF4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FG4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FH4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="FI4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FJ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FK4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FL4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="FM4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FN4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FO4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FP4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FQ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FR4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FS4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FT4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="FU4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FV4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FW4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FX4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="FY4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="FZ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GB4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GC4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GD4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GE4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GF4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GG4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GH4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GI4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GJ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GK4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GL4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GM4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GN4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GO4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GP4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GQ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GR4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GS4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GU4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GV4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GW4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="GX4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GY4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="GZ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="HA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="HB4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="HC4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="HD4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HE4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="HF4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="HG4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="HH4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HI4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="HJ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HK4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HL4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HM4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HO4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HP4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HQ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HR4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HS4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HT4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HU4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HV4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HW4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HX4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HY4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HZ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IA4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IB4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IC4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="ID4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IE4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IF4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IG4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IH4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="II4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IJ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IK4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IM4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IN4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IO4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IP4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IQ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IR4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IS4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="IT4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="IU4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="IV4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="IW4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="IX4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="IY4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="IZ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="JB4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="JC4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="JD4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JE4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="JF4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JG4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JH4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JJ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JK4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JL4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JM4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JN4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JO4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JP4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JQ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JR4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JS4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JT4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JU4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JV4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JW4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JX4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JY4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="JZ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="KA4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="KB4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="KC4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="KD4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KE4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KF4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KG4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KH4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KI4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KJ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="KK4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KL4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KM4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KN4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="KO4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KP4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KQ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KR4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KS4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KT4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KU4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KV4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="KW4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KX4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KY4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="KZ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="LB4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="LC4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="LD4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="LE4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="LF4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="LG4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="LH4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LI4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="LJ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="LK4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="LL4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LM4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="LN4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LO4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LP4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LQ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LR4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LS4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LT4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LU4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LV4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LW4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LX4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LY4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="LZ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MB4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MC4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MD4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="ME4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MF4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="MG4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MH4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MI4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MJ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="MK4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="ML4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MM4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MN4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MO4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MP4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MQ4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MR4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="MS4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MT4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MU4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MV4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="MW4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="MX4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="MY4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="MZ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NA4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NB4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NC4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="ND4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NE4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NF4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NG4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NH4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NI4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NJ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NK4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NL4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NM4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NN4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NO4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NQ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NR4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NS4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NT4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NU4" s="0" t="n">
+      <c r="B4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="V4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AD4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="AZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BD4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="BZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CD4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DD4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="DZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="ED4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="ER4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="ES4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="ET4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="EZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FD4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="FZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GD4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="GZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HD4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="ID4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="II4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="IZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JD4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="JZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KD4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="KZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LD4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="LZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MD4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="ME4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="ML4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MU4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MV4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MW4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MX4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MY4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="MZ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NA4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NB4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NC4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="ND4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NE4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NF4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NG4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NH4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NI4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NJ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NK4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NL4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NM4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NN4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NO4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NP4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NQ4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NR4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NS4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NT4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="NU4" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BT5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BU5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CB5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CE5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CI5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CJ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CK5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CL5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CM5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CN5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CP5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CQ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CR5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CS5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CT5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CU5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CV5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CW5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CX5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CY5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="CZ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="DA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DB5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DD5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="DE5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DF5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DG5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DH5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DI5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DJ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DK5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DL5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="DQ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DR5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DS5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DT5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DU5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DV5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DW5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DX5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="DY5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="DZ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EB5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="EC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="ED5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EE5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EF5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EG5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EH5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EI5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EJ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="EK5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EL5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EM5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EN5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="EO5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EP5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EQ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="ER5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="ES5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="ET5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EU5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EV5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="EW5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EX5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EY5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="EZ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="FA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FB5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FD5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FE5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FF5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FG5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FH5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="FI5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FJ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FK5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FL5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="FM5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FN5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FO5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FP5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FQ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FR5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FS5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FT5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="FU5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FV5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FW5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FX5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="FY5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="FZ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GB5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GD5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GE5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GF5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GG5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GH5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GI5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GJ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GK5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GL5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GM5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GN5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GO5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GP5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GQ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GR5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GU5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GV5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GW5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="GX5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GY5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="GZ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HB5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HD5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HE5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HF5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HG5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HH5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HI5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HJ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HK5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HL5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HM5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HO5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HP5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HQ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HR5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HS5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HT5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HU5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HV5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HW5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HX5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HY5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="HZ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IA5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IB5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IC5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="ID5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IE5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IF5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IG5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IH5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="II5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IJ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IK5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IM5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IN5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IO5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IP5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IQ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IR5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IS5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="IT5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="IU5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="IV5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="IW5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="IX5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="IY5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="IZ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="JB5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="JC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="JD5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JE5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="JF5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JG5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JH5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JJ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JK5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JL5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JM5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JN5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JO5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JP5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JQ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JR5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JS5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JT5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JU5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JV5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JW5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JX5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JY5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="JZ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="KA5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="KB5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="KC5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="KD5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KE5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KF5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KG5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KH5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KI5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KJ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="KK5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KL5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KM5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KN5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="KO5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KP5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KQ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KR5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KS5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KT5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KU5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KV5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="KW5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KX5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KY5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="KZ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="LB5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="LC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="LD5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="LE5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="LF5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="LG5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="LH5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LI5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="LJ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="LK5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="LL5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LM5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="LN5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LO5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LP5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LQ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LR5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LS5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LT5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LU5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LV5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LW5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LX5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LY5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="LZ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MB5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MC5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MD5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="ME5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MF5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="MG5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MH5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MI5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MJ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="MK5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="ML5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MM5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MN5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MO5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MP5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MQ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MR5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="MS5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MT5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MU5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MV5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="MW5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="MX5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="MY5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="MZ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NA5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NB5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NC5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="ND5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NE5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NF5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NG5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NH5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NI5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NJ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NK5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NL5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NM5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NN5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NO5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NP5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NQ5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NR5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NS5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NT5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="NU5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4785,7 +5946,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4810,7 +5971,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>